<commit_message>
added number density capability; fixed minor bugs
</commit_message>
<xml_diff>
--- a/lib/exps/c3h8_for_paper.xlsx
+++ b/lib/exps/c3h8_for_paper.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mulvihcr/PycharmProjects/pythonProject/mechsimulator/lib/exps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C45B0F-6FA9-E64E-A11C-C6AD6C245113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BF390C-E8C9-B849-8751-78CCF35872B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31280" yWindow="6200" windowWidth="22200" windowHeight="16400" xr2:uid="{E8268F29-D532-4F4A-8DC7-DD2C0037AE91}"/>
+    <workbookView xWindow="37560" yWindow="6220" windowWidth="22200" windowHeight="16400" xr2:uid="{E8268F29-D532-4F4A-8DC7-DD2C0037AE91}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>parameter</t>
   </si>
@@ -147,9 +148,6 @@
     <t>[O][O]</t>
   </si>
   <si>
-    <t>plot_format</t>
-  </si>
-  <si>
     <t>idt_targ</t>
   </si>
   <si>
@@ -189,7 +187,7 @@
     <t>CCC</t>
   </si>
   <si>
-    <t>copying from black squares in Fig. 1c</t>
+    <t>copying from black squares in Fig. 1c (phi=2.0)</t>
   </si>
 </sst>
 </file>
@@ -579,7 +577,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +639,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>20</v>
@@ -657,7 +655,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>20</v>
@@ -712,6 +710,10 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
+      <c r="H8">
+        <f>1/1.3</f>
+        <v>0.76923076923076916</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -738,13 +740,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="5">
-        <v>600</v>
+        <v>770</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="4">
+        <f>1/750</f>
+        <v>1.3333333333333333E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -754,7 +759,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5">
-        <v>680</v>
+        <v>1010</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>19</v>
@@ -770,7 +775,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="5">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>19</v>
@@ -789,7 +794,7 @@
         <v>40</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -802,10 +807,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="5">
-        <v>10</v>
+        <v>0.02</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -815,7 +820,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>12</v>
@@ -859,13 +864,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="9">
         <v>7.75</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -881,7 +886,7 @@
         <v>19.38</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -892,10 +897,10 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -906,7 +911,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="4"/>
@@ -918,10 +923,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -958,10 +963,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -994,14 +999,14 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>37</v>
+      <c r="A26" t="s">
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>

</xml_diff>